<commit_message>
added gear teeth to the gears
</commit_message>
<xml_diff>
--- a/inventor/excel/wheelParameters.xlsx
+++ b/inventor/excel/wheelParameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Inventor_Projects\AlorsBot_CAD\inventor\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB7270D3-6FFA-41F9-A4DB-49EB4E5D86E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0D28F43-4261-4765-B8D5-0A99A574666D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12585" yWindow="3855" windowWidth="14040" windowHeight="11595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="112">
   <si>
     <t>Equation</t>
   </si>
@@ -186,9 +186,6 @@
     <t>distance between gear surface and the extentions</t>
   </si>
   <si>
-    <t>IG_ratioToOuterGear</t>
-  </si>
-  <si>
     <t>Bearing Category</t>
   </si>
   <si>
@@ -355,6 +352,21 @@
   </si>
   <si>
     <t>OG_protrudeDistance</t>
+  </si>
+  <si>
+    <t>length of the slit</t>
+  </si>
+  <si>
+    <t>IG_dAxleCircleDiameter</t>
+  </si>
+  <si>
+    <t>IG_dAxleShort</t>
+  </si>
+  <si>
+    <t>IG_dAxleDepth</t>
+  </si>
+  <si>
+    <t>IG_gearRatio</t>
   </si>
 </sst>
 </file>
@@ -795,10 +807,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E63"/>
+  <dimension ref="A1:E66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -824,7 +836,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -853,7 +865,7 @@
         <v>70</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>8</v>
@@ -867,7 +879,7 @@
         <v>4</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>10</v>
@@ -881,7 +893,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>12</v>
@@ -895,7 +907,7 @@
         <v>0.3</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>14</v>
@@ -906,11 +918,11 @@
         <v>15</v>
       </c>
       <c r="B7" s="7">
-        <f>B6+B31</f>
+        <f>B6+B34</f>
         <v>5.3</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>16</v>
@@ -921,11 +933,11 @@
         <v>17</v>
       </c>
       <c r="B8" s="7">
-        <f>B17+B50*2+B6*2</f>
+        <f>B17+B53*2+B6*2</f>
         <v>10.1</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>18</v>
@@ -933,18 +945,18 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B9" s="5">
         <v>0.25</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B10" s="5">
         <v>4</v>
@@ -955,24 +967,24 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B11" s="5">
         <v>2</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B12" s="5">
         <v>0</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -995,16 +1007,16 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>51</v>
+        <v>111</v>
       </c>
       <c r="B14" s="5">
-        <v>0.75</v>
+        <v>1.25</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -1015,7 +1027,7 @@
         <v>20</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>24</v>
@@ -1029,7 +1041,7 @@
         <v>2</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>27</v>
@@ -1043,7 +1055,7 @@
         <v>7.5</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>22</v>
@@ -1054,13 +1066,13 @@
         <v>25</v>
       </c>
       <c r="B18" s="5">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E18" s="10">
         <f>B19+B20+B22</f>
@@ -1069,597 +1081,636 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B19" s="5">
         <v>10</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B20" s="5">
         <v>2</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B21" s="8">
-        <f>B28-B31</f>
-        <v>18.333333333333336</v>
+        <f>B31-B34/2*1.2</f>
+        <v>19.5</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B22" s="5">
         <v>3</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B23" s="5">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B24" s="5">
         <v>0.2</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B25" s="5">
         <v>4</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B26" s="5">
         <v>8</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B27" s="4">
-        <v>0</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E27" s="4">
-        <f>COUNTA(A28:A37)</f>
-        <v>10</v>
-      </c>
+      <c r="A27" t="s">
+        <v>108</v>
+      </c>
+      <c r="B27" s="5">
+        <v>2</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D27" s="6"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>30</v>
-      </c>
-      <c r="B28" s="8">
-        <f>B15/2+B29/2</f>
-        <v>23.333333333333336</v>
+        <v>109</v>
+      </c>
+      <c r="B28" s="5">
+        <v>1.5</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>31</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="D28" s="6"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>34</v>
-      </c>
-      <c r="B29" s="8">
-        <f>B15/B14</f>
-        <v>26.666666666666668</v>
+        <v>110</v>
+      </c>
+      <c r="B29" s="5">
+        <v>5</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D29" s="6" t="s">
-        <v>35</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="D29" s="6"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>40</v>
-      </c>
-      <c r="B30" s="5">
-        <v>2</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D30" s="6" t="s">
-        <v>41</v>
+      <c r="A30" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B30" s="4">
+        <v>0</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E30" s="4">
+        <f>COUNTA(A31:A40)</f>
+        <v>10</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>32</v>
-      </c>
-      <c r="B31" s="5">
-        <v>5</v>
+        <v>30</v>
+      </c>
+      <c r="B31" s="8">
+        <f>B15/2+B32/2</f>
+        <v>22.5</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>38</v>
-      </c>
-      <c r="B32" s="7">
-        <f>B18-B19+B5</f>
-        <v>7</v>
+        <v>34</v>
+      </c>
+      <c r="B32" s="8">
+        <f>B15*B14</f>
+        <v>25</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="B33" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>56</v>
+        <v>32</v>
       </c>
       <c r="B34" s="5">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>36</v>
-      </c>
-      <c r="B35" s="5">
-        <v>5</v>
+        <v>38</v>
+      </c>
+      <c r="B35" s="7">
+        <f>B18-B19+B5</f>
+        <v>9</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D35" t="s">
-        <v>37</v>
+        <v>58</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>107</v>
+        <v>54</v>
       </c>
       <c r="B36" s="5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="B37" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B38" s="4">
-        <v>0</v>
-      </c>
-      <c r="C38" s="4" t="s">
+      <c r="A38" t="s">
+        <v>36</v>
+      </c>
+      <c r="B38" s="5">
         <v>5</v>
       </c>
-      <c r="D38" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="E38" s="4">
-        <f>COUNTA(A39:A48)</f>
-        <v>10</v>
+      <c r="C38" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D38" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>44</v>
-      </c>
-      <c r="B39" s="7">
-        <f>B31</f>
-        <v>5</v>
+        <v>106</v>
+      </c>
+      <c r="B39" s="5">
+        <v>3</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D39" s="6" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>48</v>
-      </c>
-      <c r="B40" s="7">
-        <f>B39*0.5</f>
-        <v>2.5</v>
+        <v>74</v>
+      </c>
+      <c r="B40" s="5">
+        <v>0</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D40" s="6" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>46</v>
-      </c>
-      <c r="B41" s="8">
-        <f>B28*SQRT(2*(1-COS(RADIANS(360/B35))))-B39*5/9</f>
-        <v>24.652200662537638</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D41" s="6" t="s">
-        <v>47</v>
+      <c r="A41" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B41" s="4">
+        <v>0</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E41" s="4">
+        <f>COUNTA(A42:A51)</f>
+        <v>10</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>54</v>
-      </c>
-      <c r="B42" s="5">
-        <v>0</v>
+        <v>44</v>
+      </c>
+      <c r="B42" s="7">
+        <f>B34</f>
+        <v>5</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>77</v>
-      </c>
-      <c r="B43" s="5">
-        <v>0</v>
+        <v>48</v>
+      </c>
+      <c r="B43" s="7">
+        <f>B42*0.5</f>
+        <v>2.5</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>78</v>
-      </c>
-      <c r="B44" s="5">
-        <v>0</v>
+        <v>46</v>
+      </c>
+      <c r="B44" s="8">
+        <f>B31*SQRT(2*(1-COS(RADIANS(360/B38))))-B42*5/9</f>
+        <v>23.672558575383512</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>79</v>
+        <v>53</v>
       </c>
       <c r="B45" s="5">
         <v>0</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B46" s="5">
         <v>0</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B47" s="5">
         <v>0</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B48" s="5">
         <v>0</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="B49" s="4">
-        <v>0</v>
-      </c>
-      <c r="C49" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D49" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E49" s="4">
-        <f>COUNTA(A50:A54)</f>
-        <v>5</v>
+      <c r="A49" t="s">
+        <v>79</v>
+      </c>
+      <c r="B49" s="5">
+        <v>0</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="B50" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D50" s="6" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B51" s="5">
         <v>0</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>84</v>
-      </c>
-      <c r="B52" s="5">
-        <v>0</v>
-      </c>
-      <c r="C52" s="5" t="s">
-        <v>59</v>
+      <c r="A52" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B52" s="4">
+        <v>0</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E52" s="4">
+        <f>COUNTA(A53:A57)</f>
+        <v>5</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="B53" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
+      </c>
+      <c r="D53" s="6" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B54" s="5">
         <v>0</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="B55" s="4">
-        <v>0</v>
-      </c>
-      <c r="C55" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D55" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="E55" s="4">
-        <f>COUNTA(A56:A63)</f>
-        <v>8</v>
+      <c r="A55" t="s">
+        <v>83</v>
+      </c>
+      <c r="B55" s="5">
+        <v>0</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>97</v>
-      </c>
-      <c r="B56" s="7">
+        <v>84</v>
+      </c>
+      <c r="B56" s="5">
+        <v>0</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>85</v>
+      </c>
+      <c r="B57" s="5">
+        <v>0</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B58" s="4">
+        <v>0</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="E58" s="4">
+        <f>COUNTA(A59:A66)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>96</v>
+      </c>
+      <c r="B59" s="7">
         <f>B25-B24</f>
         <v>3.8</v>
       </c>
-      <c r="C56" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D56" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>98</v>
-      </c>
-      <c r="B57" s="7">
+      <c r="C59" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D59" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>97</v>
+      </c>
+      <c r="B60" s="7">
         <f>B26-B24</f>
         <v>7.8</v>
       </c>
-      <c r="C57" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D57" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>99</v>
-      </c>
-      <c r="B58" s="5">
-        <v>10</v>
-      </c>
-      <c r="C58" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D58" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>87</v>
-      </c>
-      <c r="B59" s="5">
-        <v>0</v>
-      </c>
-      <c r="C59" s="5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>88</v>
-      </c>
-      <c r="B60" s="5">
-        <v>0</v>
-      </c>
       <c r="C60" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
+      </c>
+      <c r="D60" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="B61" s="5">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
+      </c>
+      <c r="D61" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B62" s="5">
         <v>0</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B63" s="5">
         <v>0</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>88</v>
+      </c>
+      <c r="B64" s="5">
+        <v>0</v>
+      </c>
+      <c r="C64" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>89</v>
+      </c>
+      <c r="B65" s="5">
+        <v>0</v>
+      </c>
+      <c r="C65" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>90</v>
+      </c>
+      <c r="B66" s="5">
+        <v>0</v>
+      </c>
+      <c r="C66" s="5" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>